<commit_message>
Improved card generation, added new cards, reorganized card file structure
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
+    <sheet name="Card Drops" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Bat</t>
   </si>
@@ -114,16 +115,51 @@
   </si>
   <si>
     <t>PowerLevel</t>
+  </si>
+  <si>
+    <t>Main Spec</t>
+  </si>
+  <si>
+    <t>Off Spec</t>
+  </si>
+  <si>
+    <t>Potions</t>
+  </si>
+  <si>
+    <t>Other Specs</t>
+  </si>
+  <si>
+    <t>Relics</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>60/30/10% Main/Off/Other Stat Relic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,17 +182,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF76428A"/>
+      <color rgb="FF8F974A"/>
+      <color rgb="FFD9A066"/>
+      <color rgb="FF639BFF"/>
+      <color rgb="FF5FCDE4"/>
+      <color rgb="FFD95763"/>
+      <color rgb="FF4B692F"/>
+      <color rgb="FFAC3232"/>
+      <color rgb="FF847E87"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -433,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -999,4 +1053,112 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1">
+        <f>SUM(B1:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Class/card development, stat reworks
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -2,18 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Unity Projects\Dungeon Decks\Assets\ScriptableObjects\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
     <sheet name="Card Drops" sheetId="2" r:id="rId2"/>
+    <sheet name="Classes" sheetId="3" r:id="rId3"/>
+    <sheet name="Cards" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,8 +27,313 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Zachary Waller</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes the next Str card you use do have x more magnitude</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enemies can't see you for X turns or until you use another card</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes the next Mag card you use have x more magnitude</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Counter the next attack for X damage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes the next Str card you use do have x more magnitude</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Attack all adjacent enemies for X damage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Weapons you can attack with from an extra space away</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes the next Mag card you use have x more magnitude</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Roll 2 spaces in direction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Add all burns together. Deals half the total, and applies the rest of the damage as a DoT over the average time
+Example:
+Enemy has 3 burns:
+5 dmg over 3 turns
+2 dmg over 2 turns
+8 dmg over 4 turns
+Total dmg: 15, avg time: 3 turns
+Deal 7 dmg instantly, apply burn 8 dmg over 3 turns</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enemies can't see you for X turns or until you use another card</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Increase Main/Off stat by X for Y turns</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Bat</t>
   </si>
@@ -117,27 +425,15 @@
     <t>PowerLevel</t>
   </si>
   <si>
-    <t>Main Spec</t>
-  </si>
-  <si>
-    <t>Off Spec</t>
-  </si>
-  <si>
     <t>Potions</t>
   </si>
   <si>
-    <t>Other Specs</t>
-  </si>
-  <si>
     <t>Relics</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>60/30/10% Main/Off/Other Stat Relic</t>
-  </si>
-  <si>
     <t>DMG</t>
   </si>
   <si>
@@ -150,23 +446,152 @@
     <t>Bonus Save</t>
   </si>
   <si>
-    <t>Blocked</t>
-  </si>
-  <si>
-    <t>Broken</t>
-  </si>
-  <si>
     <t>DMG Taken</t>
   </si>
   <si>
-    <t>AP Rem</t>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>MAG</t>
+  </si>
+  <si>
+    <t>DEX</t>
+  </si>
+  <si>
+    <t>ENH</t>
+  </si>
+  <si>
+    <t>Barbarian</t>
+  </si>
+  <si>
+    <t>Magus</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Witch Hunter</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Nightblade</t>
+  </si>
+  <si>
+    <t>Monk</t>
+  </si>
+  <si>
+    <t>Shaman</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>AP Blocked</t>
+  </si>
+  <si>
+    <t>AP Broken</t>
+  </si>
+  <si>
+    <t>AP Left</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Swords</t>
+  </si>
+  <si>
+    <t>Wards</t>
+  </si>
+  <si>
+    <t>HoTs</t>
+  </si>
+  <si>
+    <t>Burns</t>
+  </si>
+  <si>
+    <t>Nukes</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Thrown</t>
+  </si>
+  <si>
+    <t>Buffs</t>
+  </si>
+  <si>
+    <t>Debuffs/Curses</t>
+  </si>
+  <si>
+    <t>Thorns</t>
+  </si>
+  <si>
+    <t>Enchant Weapon</t>
+  </si>
+  <si>
+    <t>Leather Armor</t>
+  </si>
+  <si>
+    <t>Thick Skin</t>
+  </si>
+  <si>
+    <t>Empower</t>
+  </si>
+  <si>
+    <t>Drains</t>
+  </si>
+  <si>
+    <t>Stealth</t>
+  </si>
+  <si>
+    <t>Counterattack</t>
+  </si>
+  <si>
+    <t>Heals</t>
+  </si>
+  <si>
+    <t>Whirlwind</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Cauterize</t>
+  </si>
+  <si>
+    <t>Spears</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t>45/45/10% Primary/Secondary/Other Stat Relic</t>
+  </si>
+  <si>
+    <t>40/40/20% Primary/Secondary/Mixed Decks</t>
+  </si>
+  <si>
+    <t>H Weapons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +613,89 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,17 +707,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -509,11 +1039,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1081,27 +1613,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="2" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1110,47 +1647,45 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>0.2</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
       <c r="B4" s="1"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
+        <f>SUM(B1:B3)</f>
+        <v>0.99999999999999989</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1158,89 +1693,412 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1">
-        <f>SUM(B1:B5)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>FLOOR(MIN(B12, MIN(D12, (B12 /2) + B15)),1)</f>
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <f>MAX(0, B19-C15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>15</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>MIN(B12, MIN(C12, (B12 /2) + D12))</f>
-        <v>15</v>
-      </c>
-      <c r="H12">
-        <f>MAX(0, G12-E12)</f>
-        <v>15</v>
-      </c>
-      <c r="J12">
-        <f>C12-H12</f>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f>B12-G12-IF(J12&lt;0, J12, 0)</f>
-        <v>5</v>
+      <c r="D21" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B22" s="5">
+        <f>MAX(0,(B12-B19-D15))</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="7">
+        <f>D12-D19</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="E8" sqref="E8:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="15" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="12" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="5" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new cards to card pools
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -10,7 +10,6 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -1045,7 +1044,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1619,9 +1617,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1788,9 +1783,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E8" sqref="E8:E9"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1888,10 +1880,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2002,7 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E10" s="13" t="s">
@@ -2026,7 +2015,7 @@
       <c r="D11" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2056,7 +2045,7 @@
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="10"/>

</xml_diff>

<commit_message>
Update to Unity 2017.2
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -200,7 +200,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sort of like Monk stagger in wow
+Buff that lasts 10 turns that causes damage taken to stagger out to rest of duration. Damage is rounded down, so some damage can be completely eaten by stagger
+ex:
+10 turns remaining, take a 10 damage hit
+take 1 dmg every turn for 10 turns
+5 turns remaining, take a 10 damage hit
+take 1 + 2 dmg every turn for remaining 5 turns
+ex:
+10 turns remaining, take a 15 damage hit
+15/10 = 1. So 5 damage is eaten</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -303,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0" shapeId="0">
+    <comment ref="E17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -332,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
   <si>
     <t>Bat</t>
   </si>
@@ -584,6 +617,9 @@
   </si>
   <si>
     <t>H Weapons</t>
+  </si>
+  <si>
+    <t>Stagger</t>
   </si>
 </sst>
 </file>
@@ -1877,10 +1913,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,108 +1990,106 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>75</v>
+        <v>59</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="14" t="s">
-        <v>78</v>
+      <c r="C9" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="13" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="I13" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="13" t="s">
-        <v>70</v>
-      </c>
+      <c r="D14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="11"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
       <c r="E15" s="13" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I15" s="10"/>
     </row>
@@ -2063,27 +2097,39 @@
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="E16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I21" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed health, armor, and damage to float values
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>Bat</t>
   </si>
@@ -523,9 +523,6 @@
     <t>Monk</t>
   </si>
   <si>
-    <t>Shaman</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
@@ -620,6 +617,15 @@
   </si>
   <si>
     <t>Stagger</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Battle Mage</t>
+  </si>
+  <si>
+    <t>Priest</t>
   </si>
 </sst>
 </file>
@@ -1663,13 +1669,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1">
         <v>0.7</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1696,7 +1702,7 @@
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1755,7 +1761,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1771,10 +1777,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1792,7 +1798,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -1816,8 +1822,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1866,7 @@
         <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
@@ -1870,24 +1876,28 @@
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E5" t="s">
@@ -1898,9 +1908,9 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>51</v>
       </c>
@@ -1915,8 +1925,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,54 +1954,54 @@
         <v>38</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="17"/>
@@ -2002,31 +2012,31 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -2034,7 +2044,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -2046,20 +2056,20 @@
       <c r="B11" s="8"/>
       <c r="C11" s="18"/>
       <c r="D11" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2069,14 +2079,14 @@
         <v>7</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="11"/>
       <c r="I14" s="10"/>
@@ -2089,7 +2099,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
       <c r="E15" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="10"/>
     </row>
@@ -2098,7 +2108,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="8"/>
       <c r="E16" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="10"/>
     </row>
@@ -2107,7 +2117,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="8"/>
       <c r="E17" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -2115,7 +2125,7 @@
       <c r="C18" s="20"/>
       <c r="D18" s="9"/>
       <c r="E18" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added infinite duration auras, added class special card
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,6 +220,134 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+Makes the next Mag card you use have x more magnitude</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Roll 2 spaces in direction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Add all burns together. Deals half the total, and applies the rest of the damage as a DoT over the average time
+Example:
+Enemy has 3 burns:
+5 dmg over 3 turns
+2 dmg over 2 turns
+8 dmg over 4 turns
+Total dmg: 15, avg time: 3 turns
+Deal 7 dmg instantly, apply burn 8 dmg over 3 turns</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enemies can't see you for X turns or until you use another card</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Increase Main/Off stat by X for Y turns</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Zachary Waller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Zachary Waller:
 Sort of like Monk stagger in wow
 Buff that lasts 10 turns that causes damage taken to stagger out to rest of duration. Damage is rounded down, so some damage can be completely eaten by stagger
 ex:
@@ -233,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,110 +381,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Makes the next Mag card you use have x more magnitude</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Zachary Waller:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Roll 2 spaces in direction</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Zachary Waller:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Add all burns together. Deals half the total, and applies the rest of the damage as a DoT over the average time
-Example:
-Enemy has 3 burns:
-5 dmg over 3 turns
-2 dmg over 2 turns
-8 dmg over 4 turns
-Total dmg: 15, avg time: 3 turns
-Deal 7 dmg instantly, apply burn 8 dmg over 3 turns</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Zachary Waller:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Enemies can't see you for X turns or until you use another card</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Zachary Waller:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Increase Main/Off stat by X for Y turns</t>
+Removes a harmful effect</t>
         </r>
       </text>
     </comment>
@@ -365,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t>Bat</t>
   </si>
@@ -523,6 +548,9 @@
     <t>Monk</t>
   </si>
   <si>
+    <t>Shaman</t>
+  </si>
+  <si>
     <t>DR</t>
   </si>
   <si>
@@ -626,13 +654,25 @@
   </si>
   <si>
     <t>Priest</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Cleric</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Purify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +748,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1669,13 +1722,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1">
         <v>0.7</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1702,7 +1755,7 @@
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1761,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1777,10 +1830,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1851,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -1822,8 +1875,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,7 +1919,7 @@
         <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
@@ -1877,7 +1930,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>47</v>
@@ -1886,7 +1939,7 @@
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1896,7 +1949,9 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
@@ -1908,9 +1963,15 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E6" t="s">
         <v>51</v>
       </c>
@@ -1923,10 +1984,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,152 +2015,154 @@
         <v>38</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="17"/>
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
       <c r="B7" s="8"/>
       <c r="C7" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>74</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="13" t="s">
-        <v>61</v>
+      <c r="C9" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="18"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="11"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
       <c r="E15" s="13" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I15" s="10"/>
     </row>
@@ -2108,38 +2171,32 @@
       <c r="C16" s="9"/>
       <c r="D16" s="8"/>
       <c r="E16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="10"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="13" t="s">
-        <v>64</v>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="20"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I22" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added special card ideas
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Databases/Databases.xlsx
+++ b/Assets/ScriptableObjects/Databases/Databases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -248,37 +248,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Zachary Waller:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Add all burns together. Deals half the total, and applies the rest of the damage as a DoT over the average time
-Example:
-Enemy has 3 burns:
-5 dmg over 3 turns
-2 dmg over 2 turns
-8 dmg over 4 turns
-Total dmg: 15, avg time: 3 turns
-Deal 7 dmg instantly, apply burn 8 dmg over 3 turns</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E12" authorId="0" shapeId="0">
       <text>
         <r>
@@ -390,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="111">
   <si>
     <t>Bat</t>
   </si>
@@ -666,6 +635,63 @@
   </si>
   <si>
     <t>Purify</t>
+  </si>
+  <si>
+    <t>Special Cards</t>
+  </si>
+  <si>
+    <t>Bulwark</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Leap 3 squares - Card</t>
+  </si>
+  <si>
+    <t>Take no damage for X turns - Card</t>
+  </si>
+  <si>
+    <t>Adds all burns together and deals half of total outright and applies rest as burn - Card</t>
+  </si>
+  <si>
+    <t>Staggers out all damage taken over 10 turns - Aura</t>
+  </si>
+  <si>
+    <t>Revive</t>
+  </si>
+  <si>
+    <t>Heals for half of missing health - Card</t>
+  </si>
+  <si>
+    <t>Juggernaut</t>
+  </si>
+  <si>
+    <t>Quiver</t>
+  </si>
+  <si>
+    <t>Can use ranged attacks twice before discarding - Aura</t>
+  </si>
+  <si>
+    <t>Salvage</t>
+  </si>
+  <si>
+    <t>Plus (1% max AP) AP when discarding - Aura</t>
+  </si>
+  <si>
+    <t>Conduit</t>
+  </si>
+  <si>
+    <t>Plus (1% max HP) HP when discarding - Aura</t>
+  </si>
+  <si>
+    <t>Armor cards  50% more effective - Aura</t>
   </si>
 </sst>
 </file>
@@ -868,6 +894,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H9:I18" totalsRowShown="0">
+  <autoFilter ref="H9:I18"/>
+  <sortState ref="H10:I17">
+    <sortCondition ref="H9:H17"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Card"/>
+    <tableColumn id="2" name="Effect"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1873,25 +1913,27 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="15" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
-    <col min="8" max="12" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.28515625" customWidth="1"/>
+    <col min="10" max="12" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1908,7 +1950,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1925,7 +1967,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1942,7 +1984,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1959,7 +2001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1976,8 +2018,172 @@
         <v>51</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1986,8 +2192,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2097,9 +2303,6 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="14" t="s">
-        <v>78</v>
-      </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>

</xml_diff>